<commit_message>
Partie 1 - Mise en Forme
Partie 1 - Mise en Forme

1) Nouveau template
2) Eviter les losanges et les ellipses pour les domaines très grands (plus de 200, ces formes ne sont pas incluses pour le tirage au sort)
3) Traduction en Anglais
4) Pour la Mise à Echelle, les posiions des domaines sont désormais affichées à gauche de la ligne pointillé. Cela garantit un affichage complet de la position
5) On affiche par défaut 10 protéines par page (tout si moins de 10 protéines dans le groupe)
</commit_message>
<xml_diff>
--- a/includes/excels/archs.txt.xlsx
+++ b/includes/excels/archs.txt.xlsx
@@ -928,7 +928,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="71">
+  <fonts count="72">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -951,9 +951,90 @@
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff969697"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff0f0701"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff0f0701"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff1f0001"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
       <u val="single"/>
       <sz val="11"/>
-      <color rgb="FFff232324"/>
+      <color rgb="FFffffffffff800100"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffd174a9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffff0566"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff0a0a0b"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff0a0a24"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffd0b0b1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -962,7 +1043,25 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFffffff75"/>
+      <color rgb="FFffffffffffd0b0b1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffe6e690"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff0f0010"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -971,7 +1070,16 @@
       <strike val="0"/>
       <u val="single"/>
       <sz val="11"/>
-      <color rgb="FFff0f0701"/>
+      <color rgb="FFffffffffff000020"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff887767"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -980,7 +1088,25 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff0f0001"/>
+      <color rgb="FFffffffffff001b3c"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffff4001"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff849712"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -989,7 +1115,88 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff005b00"/>
+      <color rgb="FFffffffffff050f1a"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff002900"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff7f7f80"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff0f0001"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff80002c"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffffff01"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff783115"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff117d12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff00493f"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff2d96e2"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -998,7 +1205,34 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff000001"/>
+      <color rgb="FFffffffffff45aa2d"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff1f0001"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff00102b"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff8f7f70"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1007,7 +1241,16 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff050f1a"/>
+      <color rgb="FFffffffffff3f3f40"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff007400"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1016,7 +1259,61 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff001b3c"/>
+      <color rgb="FFffffffffff000001"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff565657"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffd174a9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffb4ff7e"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff5200d1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffff0081"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff000020"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1025,7 +1322,43 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFffcd32ce"/>
+      <color rgb="FFffffffffff704371"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff99cc67"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff7f7f80"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff23ebc4"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffffff01"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1034,7 +1367,52 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff830400"/>
+      <color rgb="FFffffffffffffff01"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff001b3c"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff969697"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff4dddde"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff783106"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff8f7f70"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1043,7 +1421,97 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff191906"/>
+      <color rgb="FFffffffffffff312f"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff74baed"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffd0b0b1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff001b1f"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffffc34c8f"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff783106"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff75d41e"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff111756"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff6c8f25"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff191906"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="1"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff969697"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1052,7 +1520,16 @@
       <strike val="0"/>
       <u val="single"/>
       <sz val="11"/>
-      <color rgb="FFff7f7f80"/>
+      <color rgb="FFffffffffff255ae0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff5fadd3"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1061,34 +1538,25 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff783106"/>
+      <color rgb="FFffffffffff225f23"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFffffffffff2c2c2d"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff002900"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
       <i val="1"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff80002c"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff0a0a24"/>
+      <color rgb="FFffffffffff005b00"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1097,61 +1565,7 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFffff0081"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFffff312f"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff232324"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff000020"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff2d96e2"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff3f3f40"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff007400"/>
+      <color rgb="FFffffffffff9471dd"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1160,416 +1574,11 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FFff274028"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff8f7f70"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFffdf4d56"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff969697"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFffff7475"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff424895"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff565657"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff005b00"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff001433"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff232324"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff7f7f80"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff00ff01"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff1f0001"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff4dddde"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff005b00"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff214779"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff424895"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff00ff01"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff000020"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff783115"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff0f0701"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff327ac1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFffbe961f"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff0a214d"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff501112"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff258f2a"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff2c2c2d"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFffdf4d56"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff191906"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff8f7f70"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff4f1f1a"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff000020"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff0f0010"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff0f0701"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff05052e"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFffc34c8f"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff000a12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff000506"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff248f6d"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff232324"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff000533"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff002547"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFffff9c00"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff969697"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FFff887767"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="1"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFff95a533"/>
+      <color rgb="FFffffffffffd174a9"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="56">
+  <fills count="58">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1587,14 +1596,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDCDCDC&#13;&#10;"/>
-        <bgColor rgb="FFDCDCDC&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00008B&#13;&#10;"/>
-        <bgColor rgb="FF00008B&#13;&#10;"/>
+        <fgColor rgb="FF696969&#13;&#10;"/>
+        <bgColor rgb="FF696969&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1605,20 +1608,86 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFFF&#13;&#10;"/>
-        <bgColor rgb="FFF0FFFF&#13;&#10;"/>
+        <fgColor rgb="FFE0FFFF&#13;&#10;"/>
+        <bgColor rgb="FFE0FFFF&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500&#13;&#10;"/>
-        <bgColor rgb="FFFFA500&#13;&#10;"/>
+        <fgColor rgb="FF7FFF00&#13;&#10;"/>
+        <bgColor rgb="FF7FFF00&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF&#13;&#10;"/>
-        <bgColor rgb="FFFFFFFF&#13;&#10;"/>
+        <fgColor rgb="FF2E8B57&#13;&#10;"/>
+        <bgColor rgb="FF2E8B57&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FA9A&#13;&#10;"/>
+        <bgColor rgb="FF00FA9A&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5&#13;&#10;"/>
+        <bgColor rgb="FFF5F5F5&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5DC&#13;&#10;"/>
+        <bgColor rgb="FFF5F5DC&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2F4F4F&#13;&#10;"/>
+        <bgColor rgb="FF2F4F4F&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF191970&#13;&#10;"/>
+        <bgColor rgb="FF191970&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0FFF0&#13;&#10;"/>
+        <bgColor rgb="FFF0FFF0&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFE0&#13;&#10;"/>
+        <bgColor rgb="FFFFFFE0&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF778899&#13;&#10;"/>
+        <bgColor rgb="FF778899&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE4C4&#13;&#10;"/>
+        <bgColor rgb="FFFFE4C4&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00BFFF&#13;&#10;"/>
+        <bgColor rgb="FF00BFFF&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7B68EE&#13;&#10;"/>
+        <bgColor rgb="FF7B68EE&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1629,26 +1698,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE4C4&#13;&#10;"/>
-        <bgColor rgb="FFFFE4C4&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF32CD32&#13;&#10;"/>
-        <bgColor rgb="FF32CD32&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7CFC00&#13;&#10;"/>
-        <bgColor rgb="FF7CFC00&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6FA&#13;&#10;"/>
-        <bgColor rgb="FFE6E6FA&#13;&#10;"/>
+        <fgColor rgb="FFFFD700&#13;&#10;"/>
+        <bgColor rgb="FFFFD700&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1659,14 +1710,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF87CEFA&#13;&#10;"/>
-        <bgColor rgb="FF87CEFA&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD700&#13;&#10;"/>
-        <bgColor rgb="FFFFD700&#13;&#10;"/>
+        <fgColor rgb="FFF0FFFF&#13;&#10;"/>
+        <bgColor rgb="FFF0FFFF&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1677,32 +1722,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5F5DC&#13;&#10;"/>
-        <bgColor rgb="FFF5F5DC&#13;&#10;"/>
+        <fgColor rgb="FF0000FF&#13;&#10;"/>
+        <bgColor rgb="FF0000FF&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF7F&#13;&#10;"/>
-        <bgColor rgb="FF00FF7F&#13;&#10;"/>
+        <fgColor rgb="FF87CEEB&#13;&#10;"/>
+        <bgColor rgb="FF87CEEB&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CED1&#13;&#10;"/>
-        <bgColor rgb="FF00CED1&#13;&#10;"/>
+        <fgColor rgb="FFEE82EE&#13;&#10;"/>
+        <bgColor rgb="FFEE82EE&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFE0&#13;&#10;"/>
-        <bgColor rgb="FFFFFFE0&#13;&#10;"/>
+        <fgColor rgb="FFFFB6C1&#13;&#10;"/>
+        <bgColor rgb="FFFFB6C1&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD2691E&#13;&#10;"/>
         <bgColor rgb="FFD2691E&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBA55D3&#13;&#10;"/>
+        <bgColor rgb="FFBA55D3&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEFD5&#13;&#10;"/>
+        <bgColor rgb="FFFFEFD5&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF708090&#13;&#10;"/>
+        <bgColor rgb="FF708090&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1719,38 +1782,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD8BFD8&#13;&#10;"/>
-        <bgColor rgb="FFD8BFD8&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF708090&#13;&#10;"/>
-        <bgColor rgb="FF708090&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF20B2AA&#13;&#10;"/>
-        <bgColor rgb="FF20B2AA&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF696969&#13;&#10;"/>
-        <bgColor rgb="FF696969&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008B8B&#13;&#10;"/>
-        <bgColor rgb="FF008B8B&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBDB76B&#13;&#10;"/>
-        <bgColor rgb="FFBDB76B&#13;&#10;"/>
+        <fgColor rgb="FFFFFFFF&#13;&#10;"/>
+        <bgColor rgb="FFFFFFFF&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1761,20 +1794,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEBCD&#13;&#10;"/>
-        <bgColor rgb="FFFFEBCD&#13;&#10;"/>
+        <fgColor rgb="FF4B0082&#13;&#10;"/>
+        <bgColor rgb="FF4B0082&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF&#13;&#10;"/>
-        <bgColor rgb="FFFF00FF&#13;&#10;"/>
+        <fgColor rgb="FFADFF2F&#13;&#10;"/>
+        <bgColor rgb="FFADFF2F&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE0FFFF&#13;&#10;"/>
-        <bgColor rgb="FFE0FFFF&#13;&#10;"/>
+        <fgColor rgb="FF00FF7F&#13;&#10;"/>
+        <bgColor rgb="FF00FF7F&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FBC8F&#13;&#10;"/>
+        <bgColor rgb="FF8FBC8F&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF663399&#13;&#10;"/>
+        <bgColor rgb="FF663399&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDC143C&#13;&#10;"/>
+        <bgColor rgb="FFDC143C&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1785,44 +1836,74 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDEB887&#13;&#10;"/>
-        <bgColor rgb="FFDEB887&#13;&#10;"/>
+        <fgColor rgb="FF87CEFA&#13;&#10;"/>
+        <bgColor rgb="FF87CEFA&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF87CEEB&#13;&#10;"/>
-        <bgColor rgb="FF87CEEB&#13;&#10;"/>
+        <fgColor rgb="FF00CED1&#13;&#10;"/>
+        <bgColor rgb="FF00CED1&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCD853F&#13;&#10;"/>
-        <bgColor rgb="FFCD853F&#13;&#10;"/>
+        <fgColor rgb="FF8B4513&#13;&#10;"/>
+        <bgColor rgb="FF8B4513&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4169E1&#13;&#10;"/>
-        <bgColor rgb="FF4169E1&#13;&#10;"/>
+        <fgColor rgb="FFFFE4E1&#13;&#10;"/>
+        <bgColor rgb="FFFFE4E1&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5DEB3&#13;&#10;"/>
-        <bgColor rgb="FFF5DEB3&#13;&#10;"/>
+        <fgColor rgb="FF3CB371&#13;&#10;"/>
+        <bgColor rgb="FF3CB371&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAFEEEE&#13;&#10;"/>
-        <bgColor rgb="FFAFEEEE&#13;&#10;"/>
+        <fgColor rgb="FF8A2BE2&#13;&#10;"/>
+        <bgColor rgb="FF8A2BE2&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDA70D6&#13;&#10;"/>
-        <bgColor rgb="FFDA70D6&#13;&#10;"/>
+        <fgColor rgb="FFEEE8AA&#13;&#10;"/>
+        <bgColor rgb="FFEEE8AA&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9370DB&#13;&#10;"/>
+        <bgColor rgb="FF9370DB&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6FA&#13;&#10;"/>
+        <bgColor rgb="FFE6E6FA&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAA520&#13;&#10;"/>
+        <bgColor rgb="FFDAA520&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA0522D&#13;&#10;"/>
+        <bgColor rgb="FFA0522D&#13;&#10;"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDA0DD&#13;&#10;"/>
+        <bgColor rgb="FFDDA0DD&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
@@ -1833,74 +1914,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB0E0E6&#13;&#10;"/>
-        <bgColor rgb="FFB0E0E6&#13;&#10;"/>
+        <fgColor rgb="FFFFA500&#13;&#10;"/>
+        <bgColor rgb="FFFFA500&#13;&#10;"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFF0&#13;&#10;"/>
-        <bgColor rgb="FFF0FFF0&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFAFAD2&#13;&#10;"/>
-        <bgColor rgb="FFFAFAD2&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3CB371&#13;&#10;"/>
-        <bgColor rgb="FF3CB371&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF5EE&#13;&#10;"/>
-        <bgColor rgb="FFFFF5EE&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFAFA&#13;&#10;"/>
-        <bgColor rgb="FFFFFAFA&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDB7093&#13;&#10;"/>
-        <bgColor rgb="FFDB7093&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFACD&#13;&#10;"/>
-        <bgColor rgb="FFFFFACD&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFDAB9&#13;&#10;"/>
-        <bgColor rgb="FFFFDAB9&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF006400&#13;&#10;"/>
-        <bgColor rgb="FF006400&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF778899&#13;&#10;"/>
-        <bgColor rgb="FF778899&#13;&#10;"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6A5ACD&#13;&#10;"/>
-        <bgColor rgb="FF6A5ACD&#13;&#10;"/>
+        <fgColor rgb="FF6B8E23&#13;&#10;"/>
+        <bgColor rgb="FF6B8E23&#13;&#10;"/>
       </patternFill>
     </fill>
   </fills>
@@ -1908,975 +1929,936 @@
     <border/>
     <border>
       <left style="double">
-        <color rgb="FFDCDCDC&#13;&#10;"/>
+        <color rgb="FF00FF7F&#13;&#10;"/>
       </left>
       <right style="double">
-        <color rgb="FFDCDCDC&#13;&#10;"/>
+        <color rgb="FF00FF7F&#13;&#10;"/>
       </right>
       <top style="double">
-        <color rgb="FFDCDCDC&#13;&#10;"/>
+        <color rgb="FF00FF7F&#13;&#10;"/>
       </top>
       <bottom style="double">
-        <color rgb="FFDCDCDC&#13;&#10;"/>
+        <color rgb="FF00FF7F&#13;&#10;"/>
       </bottom>
     </border>
     <border>
-      <left style="slantDashDot">
-        <color rgb="FFD8BFD8&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FFD8BFD8&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FFD8BFD8&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FFD8BFD8&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="mediumDashed">
+      <left style="medium">
         <color rgb="FFA52A2A&#13;&#10;"/>
       </left>
-      <right style="mediumDashed">
+      <right style="medium">
         <color rgb="FFA52A2A&#13;&#10;"/>
       </right>
-      <top style="mediumDashed">
+      <top style="medium">
         <color rgb="FFA52A2A&#13;&#10;"/>
       </top>
-      <bottom style="mediumDashed">
+      <bottom style="medium">
         <color rgb="FFA52A2A&#13;&#10;"/>
       </bottom>
     </border>
+    <border/>
     <border>
-      <left style="thick">
-        <color rgb="FFFAFAD2&#13;&#10;"/>
+      <left style="slantDashDot">
+        <color rgb="FFFFC0CB&#13;&#10;"/>
       </left>
-      <right style="thick">
-        <color rgb="FFFAFAD2&#13;&#10;"/>
+      <right style="slantDashDot">
+        <color rgb="FFFFC0CB&#13;&#10;"/>
       </right>
-      <top style="thick">
-        <color rgb="FFFAFAD2&#13;&#10;"/>
+      <top style="slantDashDot">
+        <color rgb="FFFFC0CB&#13;&#10;"/>
       </top>
-      <bottom style="thick">
-        <color rgb="FFFAFAD2&#13;&#10;"/>
+      <bottom style="slantDashDot">
+        <color rgb="FFFFC0CB&#13;&#10;"/>
       </bottom>
     </border>
     <border/>
     <border>
       <left style="thick">
+        <color rgb="FF708090&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF708090&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF708090&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF708090&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFFF0000&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFFF0000&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFFF0000&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF778899&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF778899&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF778899&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF778899&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF8B0000&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF8B0000&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF8B0000&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF8B0000&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFF5DEB3&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF5DEB3&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF5DEB3&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF5DEB3&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FFFFFAFA&#13;&#10;"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FFFFFAFA&#13;&#10;"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FFFFFAFA&#13;&#10;"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFFFFAFA&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFFFFF00&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFFFFF00&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFFFFF00&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFFFF00&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border/>
+    <border>
+      <left style="dashDot">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </left>
+      <right style="dashDot">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </right>
+      <top style="dashDot">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </top>
+      <bottom style="dashDot">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF808000&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF808000&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF808000&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF808000&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFA500&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFA500&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFA500&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFA500&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF40E0D0&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border/>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color rgb="FF483D8B&#13;&#10;"/>
+      </left>
+      <right style="dashDot">
+        <color rgb="FF483D8B&#13;&#10;"/>
+      </right>
+      <top style="dashDot">
+        <color rgb="FF483D8B&#13;&#10;"/>
+      </top>
+      <bottom style="dashDot">
+        <color rgb="FF483D8B&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFE9967A&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFE9967A&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFE9967A&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFE9967A&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF8A2BE2&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF8A2BE2&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF8A2BE2&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF8A2BE2&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="dashDot">
         <color rgb="FF00BFFF&#13;&#10;"/>
       </left>
-      <right style="thick">
+      <right style="dashDot">
         <color rgb="FF00BFFF&#13;&#10;"/>
       </right>
-      <top style="thick">
+      <top style="dashDot">
         <color rgb="FF00BFFF&#13;&#10;"/>
       </top>
-      <bottom style="thick">
+      <bottom style="dashDot">
         <color rgb="FF00BFFF&#13;&#10;"/>
       </bottom>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF8B0000&#13;&#10;"/>
+      <left style="hair">
+        <color rgb="FF9ACD32"/>
       </left>
-      <right style="double">
-        <color rgb="FF8B0000&#13;&#10;"/>
+      <right style="hair">
+        <color rgb="FF9ACD32"/>
       </right>
-      <top style="double">
-        <color rgb="FF8B0000&#13;&#10;"/>
+      <top style="hair">
+        <color rgb="FF9ACD32"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF8B0000&#13;&#10;"/>
+      <bottom style="hair">
+        <color rgb="FF9ACD32"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF191970&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF191970&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF191970&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF191970&#13;&#10;"/>
       </bottom>
     </border>
     <border/>
     <border>
       <left style="mediumDashed">
+        <color rgb="FF708090&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF708090&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF708090&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF708090&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF87CEFA&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FF87CEFA&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FF87CEFA&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF87CEFA&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFFF4500&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFFF4500&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFFF4500&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF4500&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border/>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFE4B5&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFE4B5&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFE4B5&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFE4B5&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFB8860B&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border/>
+    <border>
+      <left style="hair">
+        <color rgb="FF7FFF00&#13;&#10;"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF7FFF00&#13;&#10;"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF7FFF00&#13;&#10;"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF7FFF00&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFE0FFFF&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFE0FFFF&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFE0FFFF&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFE0FFFF&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF9932CC&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF9932CC&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF9932CC&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF9932CC&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8B008B&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF8B008B&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF8B008B&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8B008B&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFD8BFD8&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFD8BFD8&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFD8BFD8&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFD8BFD8&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF0000FF&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FF66CDAA&#13;&#10;"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FF66CDAA&#13;&#10;"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FF66CDAA&#13;&#10;"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FF66CDAA&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FFD2B48C&#13;&#10;"/>
       </left>
-      <right style="mediumDashed">
+      <right style="medium">
         <color rgb="FFD2B48C&#13;&#10;"/>
       </right>
-      <top style="mediumDashed">
+      <top style="medium">
         <color rgb="FFD2B48C&#13;&#10;"/>
       </top>
-      <bottom style="mediumDashed">
+      <bottom style="medium">
         <color rgb="FFD2B48C&#13;&#10;"/>
       </bottom>
     </border>
     <border>
       <left style="medium">
+        <color rgb="FF228B22&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF228B22&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF228B22&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF228B22&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFFDEAD&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF7B68EE&#13;&#10;"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF7B68EE&#13;&#10;"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF7B68EE&#13;&#10;"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF7B68EE&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFF4A460&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="slantDashDot">
+        <color rgb="FFDCDCDC&#13;&#10;"/>
+      </left>
+      <right style="slantDashDot">
+        <color rgb="FFDCDCDC&#13;&#10;"/>
+      </right>
+      <top style="slantDashDot">
+        <color rgb="FFDCDCDC&#13;&#10;"/>
+      </top>
+      <bottom style="slantDashDot">
+        <color rgb="FFDCDCDC&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF696969&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF696969&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF696969&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF696969&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF008B8B&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF008B8B&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF008B8B&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF008B8B&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color rgb="FFFAFAD2&#13;&#10;"/>
+      </left>
+      <right style="dashDot">
+        <color rgb="FFFAFAD2&#13;&#10;"/>
+      </right>
+      <top style="dashDot">
+        <color rgb="FFFAFAD2&#13;&#10;"/>
+      </top>
+      <bottom style="dashDot">
+        <color rgb="FFFAFAD2&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFE0&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color rgb="FFFFDAB9&#13;&#10;"/>
+      </left>
+      <right style="dashDot">
+        <color rgb="FFFFDAB9&#13;&#10;"/>
+      </right>
+      <top style="dashDot">
+        <color rgb="FFFFDAB9&#13;&#10;"/>
+      </top>
+      <bottom style="dashDot">
+        <color rgb="FFFFDAB9&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FFBC8F8F&#13;&#10;"/>
+      </left>
+      <right style="hair">
+        <color rgb="FFBC8F8F&#13;&#10;"/>
+      </right>
+      <top style="hair">
+        <color rgb="FFBC8F8F&#13;&#10;"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FFBC8F8F&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFDF5E6&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFDF5E6&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFDF5E6&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFDF5E6&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF4682B4&#13;&#10;"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF4682B4&#13;&#10;"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF4682B4&#13;&#10;"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF4682B4&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF4169E1&#13;&#10;"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF4169E1&#13;&#10;"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF4169E1&#13;&#10;"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF4169E1&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FFB0E0E6&#13;&#10;"/>
       </left>
-      <right style="medium">
+      <right style="double">
         <color rgb="FFB0E0E6&#13;&#10;"/>
       </right>
-      <top style="medium">
+      <top style="double">
         <color rgb="FFB0E0E6&#13;&#10;"/>
       </top>
-      <bottom style="medium">
+      <bottom style="double">
         <color rgb="FFB0E0E6&#13;&#10;"/>
       </bottom>
     </border>
     <border>
       <left style="slantDashDot">
-        <color rgb="FFD2691E&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </left>
       <right style="slantDashDot">
-        <color rgb="FFD2691E&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </right>
       <top style="slantDashDot">
-        <color rgb="FFD2691E&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </top>
       <bottom style="slantDashDot">
-        <color rgb="FFD2691E&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF228B22&#13;&#10;"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF228B22&#13;&#10;"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF228B22&#13;&#10;"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF228B22&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </left>
-      <right style="dashDot">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </right>
-      <top style="dashDot">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </top>
-      <bottom style="dashDot">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color rgb="FF98FB98&#13;&#10;"/>
-      </left>
-      <right style="dashDot">
-        <color rgb="FF98FB98&#13;&#10;"/>
-      </right>
-      <top style="dashDot">
-        <color rgb="FF98FB98&#13;&#10;"/>
-      </top>
-      <bottom style="dashDot">
-        <color rgb="FF98FB98&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </bottom>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFFFFFFF&#13;&#10;"/>
+        <color rgb="FFF5F5F5&#13;&#10;"/>
       </left>
       <right style="medium">
-        <color rgb="FFFFFFFF&#13;&#10;"/>
+        <color rgb="FFF5F5F5&#13;&#10;"/>
       </right>
       <top style="medium">
-        <color rgb="FFFFFFFF&#13;&#10;"/>
+        <color rgb="FFF5F5F5&#13;&#10;"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFFFFFFF&#13;&#10;"/>
+        <color rgb="FFF5F5F5&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF808080&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF808080&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF808080&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF808080&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFD3D3D3&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFD3D3D3&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFD3D3D3&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFD3D3D3&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF000080&#13;&#10;"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF000080&#13;&#10;"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF000080&#13;&#10;"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF000080&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF6A5ACD&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FFDEB887&#13;&#10;"/>
+      </left>
+      <right style="double">
+        <color rgb="FFDEB887&#13;&#10;"/>
+      </right>
+      <top style="double">
+        <color rgb="FFDEB887&#13;&#10;"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFDEB887&#13;&#10;"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF66CDAA&#13;&#10;"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF66CDAA&#13;&#10;"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF66CDAA&#13;&#10;"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF66CDAA&#13;&#10;"/>
       </bottom>
     </border>
     <border>
       <left style="slantDashDot">
-        <color rgb="FF6B8E23&#13;&#10;"/>
+        <color rgb="FF32CD32&#13;&#10;"/>
       </left>
       <right style="slantDashDot">
-        <color rgb="FF6B8E23&#13;&#10;"/>
+        <color rgb="FF32CD32&#13;&#10;"/>
       </right>
       <top style="slantDashDot">
-        <color rgb="FF6B8E23&#13;&#10;"/>
+        <color rgb="FF32CD32&#13;&#10;"/>
       </top>
       <bottom style="slantDashDot">
-        <color rgb="FF6B8E23&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border/>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FF808080&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FF808080&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FF808080&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FF808080&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF5F9EA0&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF5F9EA0&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF5F9EA0&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF5F9EA0&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FFF0FFF0&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FFF0FFF0&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FFF0FFF0&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FFF0FFF0&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FFFDF5E6&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FFFDF5E6&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FFFDF5E6&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFFDF5E6&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF808000&#13;&#10;"/>
-      </left>
-      <right style="double">
-        <color rgb="FF808000&#13;&#10;"/>
-      </right>
-      <top style="double">
-        <color rgb="FF808000&#13;&#10;"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF808000&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF7B68EE&#13;&#10;"/>
-      </left>
-      <right style="double">
-        <color rgb="FF7B68EE&#13;&#10;"/>
-      </right>
-      <top style="double">
-        <color rgb="FF7B68EE&#13;&#10;"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF7B68EE&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FFF5FFFA&#13;&#10;"/>
-      </left>
-      <right style="double">
-        <color rgb="FFF5FFFA&#13;&#10;"/>
-      </right>
-      <top style="double">
-        <color rgb="FFF5FFFA&#13;&#10;"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FFF5FFFA&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000&#13;&#10;"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000&#13;&#10;"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000&#13;&#10;"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FFFFE4B5&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FFFFE4B5&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FFFFE4B5&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFFFE4B5&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color rgb="FF6B8E23&#13;&#10;"/>
-      </left>
-      <right style="mediumDashed">
-        <color rgb="FF6B8E23&#13;&#10;"/>
-      </right>
-      <top style="mediumDashed">
-        <color rgb="FF6B8E23&#13;&#10;"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color rgb="FF6B8E23&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color rgb="FFBC8F8F&#13;&#10;"/>
-      </left>
-      <right style="mediumDashed">
-        <color rgb="FFBC8F8F&#13;&#10;"/>
-      </right>
-      <top style="mediumDashed">
-        <color rgb="FFBC8F8F&#13;&#10;"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color rgb="FFBC8F8F&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </left>
-      <right style="mediumDashed">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </right>
-      <top style="mediumDashed">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCD853F&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCD853F&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCD853F&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCD853F&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </left>
-      <right style="dashDot">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </right>
-      <top style="dashDot">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </top>
-      <bottom style="dashDot">
-        <color rgb="FF20B2AA&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color rgb="FFFFE4E1&#13;&#10;"/>
-      </left>
-      <right style="dashDot">
-        <color rgb="FFFFE4E1&#13;&#10;"/>
-      </right>
-      <top style="dashDot">
-        <color rgb="FFFFE4E1&#13;&#10;"/>
-      </top>
-      <bottom style="dashDot">
-        <color rgb="FFFFE4E1&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FFF5F5F5&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FFF5F5F5&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FFF5F5F5&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FFF5F5F5&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFA9A9A9&#13;&#10;"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFA9A9A9&#13;&#10;"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFA9A9A9&#13;&#10;"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFA9A9A9&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border/>
-    <border>
-      <left style="thick">
-        <color rgb="FF7CFC00&#13;&#10;"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF7CFC00&#13;&#10;"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF7CFC00&#13;&#10;"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF7CFC00&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color rgb="FFFFEBCD&#13;&#10;"/>
-      </left>
-      <right style="mediumDashed">
-        <color rgb="FFFFEBCD&#13;&#10;"/>
-      </right>
-      <top style="mediumDashed">
-        <color rgb="FFFFEBCD&#13;&#10;"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color rgb="FFFFEBCD&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FFDC143C&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FFDC143C&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FFDC143C&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FFDC143C&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFFF69B4&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FFC0C0C0&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FFC0C0C0&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FFC0C0C0&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFC0C0C0&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF708090&#13;&#10;"/>
-      </left>
-      <right style="double">
-        <color rgb="FF708090&#13;&#10;"/>
-      </right>
-      <top style="double">
-        <color rgb="FF708090&#13;&#10;"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF708090&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF00008B&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF00008B&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF00008B&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF00008B&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFC0CB&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFFC0CB&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFFC0CB&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFFC0CB&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color rgb="FF000080&#13;&#10;"/>
-      </left>
-      <right style="dashDot">
-        <color rgb="FF000080&#13;&#10;"/>
-      </right>
-      <top style="dashDot">
-        <color rgb="FF000080&#13;&#10;"/>
-      </top>
-      <bottom style="dashDot">
-        <color rgb="FF000080&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FFFFA500&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FFFFA500&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FFFFA500&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FFFFA500&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF4682B4&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFF4A460&#13;&#10;"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFF4A460&#13;&#10;"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFF4A460&#13;&#10;"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFF4A460&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF98FB98&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF98FB98&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF98FB98&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF98FB98&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF8B4513&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF8B4513&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF8B4513&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF8B4513&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color rgb="FF32CD32&#13;&#10;"/>
-      </left>
-      <right style="dashDot">
-        <color rgb="FF32CD32&#13;&#10;"/>
-      </right>
-      <top style="dashDot">
-        <color rgb="FF32CD32&#13;&#10;"/>
-      </top>
-      <bottom style="dashDot">
         <color rgb="FF32CD32&#13;&#10;"/>
       </bottom>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFFA8072&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </left>
       <right style="medium">
-        <color rgb="FFFA8072&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </right>
       <top style="medium">
-        <color rgb="FFFA8072&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFFA8072&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF696969&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF696969&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF696969&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF696969&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color rgb="FFFFA07A&#13;&#10;"/>
-      </left>
-      <right style="mediumDashed">
-        <color rgb="FFFFA07A&#13;&#10;"/>
-      </right>
-      <top style="mediumDashed">
-        <color rgb="FFFFA07A&#13;&#10;"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color rgb="FFFFA07A&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FFFF00FF&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FFFF00FF&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FFFF00FF&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFFF00FF&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FFFAEBD7&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FFFAEBD7&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FFFAEBD7&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FFFAEBD7&#13;&#10;"/>
+        <color rgb="FF2F4F4F&#13;&#10;"/>
       </bottom>
     </border>
     <border>
       <left style="dashDot">
-        <color rgb="FFFF00FF&#13;&#10;"/>
+        <color rgb="FFF0FFF0&#13;&#10;"/>
       </left>
       <right style="dashDot">
-        <color rgb="FFFF00FF&#13;&#10;"/>
+        <color rgb="FFF0FFF0&#13;&#10;"/>
       </right>
       <top style="dashDot">
-        <color rgb="FFFF00FF&#13;&#10;"/>
+        <color rgb="FFF0FFF0&#13;&#10;"/>
       </top>
       <bottom style="dashDot">
-        <color rgb="FFFF00FF&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF9ACD32"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF9ACD32"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF9ACD32"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF9ACD32"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color rgb="FFADD8E6&#13;&#10;"/>
-      </left>
-      <right style="slantDashDot">
-        <color rgb="FFADD8E6&#13;&#10;"/>
-      </right>
-      <top style="slantDashDot">
-        <color rgb="FFADD8E6&#13;&#10;"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color rgb="FFADD8E6&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF9370DB&#13;&#10;"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF9370DB&#13;&#10;"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF9370DB&#13;&#10;"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF9370DB&#13;&#10;"/>
+        <color rgb="FFF0FFF0&#13;&#10;"/>
       </bottom>
     </border>
     <border>
       <left style="dashDot">
-        <color rgb="FF2E8B57&#13;&#10;"/>
+        <color rgb="FFFFF0F5&#13;&#10;"/>
       </left>
       <right style="dashDot">
-        <color rgb="FF2E8B57&#13;&#10;"/>
+        <color rgb="FFFFF0F5&#13;&#10;"/>
       </right>
       <top style="dashDot">
-        <color rgb="FF2E8B57&#13;&#10;"/>
+        <color rgb="FFFFF0F5&#13;&#10;"/>
       </top>
       <bottom style="dashDot">
-        <color rgb="FF2E8B57&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF778899&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF778899&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF778899&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF778899&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF556B2F&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF556B2F&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF556B2F&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF556B2F&#13;&#10;"/>
+        <color rgb="FFFFF0F5&#13;&#10;"/>
       </bottom>
     </border>
     <border/>
-    <border>
-      <left style="medium">
-        <color rgb="FFADFF2F&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFADFF2F&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFADFF2F&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFADFF2F&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF808080&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF808080&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF808080&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF808080&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFF0000&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFF0000&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFF0000&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFF7F50&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF7F50&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFF7F50&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFF7F50&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFFFDAB9&#13;&#10;"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFFFDAB9&#13;&#10;"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFFFDAB9&#13;&#10;"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFFDAB9&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFB0C4DE&#13;&#10;"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFB0C4DE&#13;&#10;"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFB0C4DE&#13;&#10;"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFB0C4DE&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color rgb="FFFFB6C1&#13;&#10;"/>
-      </left>
-      <right style="mediumDashed">
-        <color rgb="FFFFB6C1&#13;&#10;"/>
-      </right>
-      <top style="mediumDashed">
-        <color rgb="FFFFB6C1&#13;&#10;"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color rgb="FFFFB6C1&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF008B8B&#13;&#10;"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color rgb="FFF5DEB3&#13;&#10;"/>
-      </left>
-      <right style="dashDot">
-        <color rgb="FFF5DEB3&#13;&#10;"/>
-      </right>
-      <top style="dashDot">
-        <color rgb="FFF5DEB3&#13;&#10;"/>
-      </top>
-      <bottom style="dashDot">
-        <color rgb="FFF5DEB3&#13;&#10;"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2894,226 +2876,226 @@
     <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="5" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="6" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="5" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="7" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="6" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="7" numFmtId="0" fillId="8" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="4" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="8" numFmtId="0" fillId="9" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="7" numFmtId="0" fillId="7" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="9" numFmtId="0" fillId="10" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="8" numFmtId="0" fillId="8" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="10" numFmtId="0" fillId="11" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="9" numFmtId="0" fillId="9" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="11" numFmtId="0" fillId="12" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="10" numFmtId="0" fillId="10" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="12" numFmtId="0" fillId="13" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="11" numFmtId="0" fillId="11" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="13" numFmtId="0" fillId="14" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="12" numFmtId="0" fillId="11" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="14" numFmtId="0" fillId="15" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="13" numFmtId="0" fillId="12" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="15" numFmtId="0" fillId="16" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="14" numFmtId="0" fillId="13" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="16" numFmtId="0" fillId="17" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="15" numFmtId="0" fillId="14" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="17" numFmtId="0" fillId="18" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="16" numFmtId="0" fillId="15" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="18" numFmtId="0" fillId="19" borderId="17" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="17" numFmtId="0" fillId="16" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="19" numFmtId="0" fillId="20" borderId="18" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="18" numFmtId="0" fillId="17" borderId="17" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="15" numFmtId="0" fillId="16" borderId="19" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="19" numFmtId="0" fillId="18" borderId="18" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="20" numFmtId="0" fillId="3" borderId="20" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="20" numFmtId="0" fillId="19" borderId="19" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="21" numFmtId="0" fillId="21" borderId="21" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="21" numFmtId="0" fillId="20" borderId="20" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="22" numFmtId="0" fillId="22" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="22" numFmtId="0" fillId="21" borderId="21" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="23" numFmtId="0" fillId="23" borderId="23" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="20" numFmtId="0" fillId="19" borderId="22" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="24" numFmtId="0" fillId="24" borderId="24" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="23" numFmtId="0" fillId="22" borderId="23" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="25" numFmtId="0" fillId="25" borderId="25" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="24" numFmtId="0" fillId="23" borderId="24" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="26" numFmtId="0" fillId="26" borderId="26" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="25" numFmtId="0" fillId="24" borderId="25" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="27" numFmtId="0" fillId="27" borderId="27" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="26" numFmtId="0" fillId="25" borderId="26" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="28" numFmtId="0" fillId="28" borderId="28" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="27" numFmtId="0" fillId="26" borderId="27" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="29" numFmtId="0" fillId="29" borderId="29" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="28" numFmtId="0" fillId="27" borderId="28" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="30" numFmtId="0" fillId="30" borderId="30" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="29" numFmtId="0" fillId="28" borderId="29" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="31" numFmtId="0" fillId="31" borderId="31" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="30" numFmtId="0" fillId="29" borderId="30" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="32" numFmtId="0" fillId="7" borderId="32" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="31" numFmtId="0" fillId="5" borderId="31" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="33" numFmtId="0" fillId="32" borderId="33" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="32" numFmtId="0" fillId="30" borderId="32" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="34" numFmtId="0" fillId="3" borderId="34" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="33" numFmtId="0" fillId="31" borderId="33" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="35" numFmtId="0" fillId="14" borderId="35" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="34" numFmtId="0" fillId="32" borderId="34" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="36" numFmtId="0" fillId="33" borderId="36" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="35" numFmtId="0" fillId="33" borderId="35" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="37" numFmtId="0" fillId="34" borderId="37" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="36" numFmtId="0" fillId="34" borderId="36" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="38" numFmtId="0" fillId="35" borderId="38" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="37" numFmtId="0" fillId="35" borderId="37" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="39" numFmtId="0" fillId="7" borderId="39" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="38" numFmtId="0" fillId="7" borderId="38" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="40" numFmtId="0" fillId="36" borderId="40" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="39" numFmtId="0" fillId="36" borderId="39" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="41" numFmtId="0" fillId="30" borderId="35" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="40" numFmtId="0" fillId="37" borderId="40" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="42" numFmtId="0" fillId="33" borderId="41" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="41" numFmtId="0" fillId="38" borderId="41" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="43" numFmtId="0" fillId="21" borderId="42" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="42" numFmtId="0" fillId="14" borderId="42" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="44" numFmtId="0" fillId="37" borderId="43" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="43" numFmtId="0" fillId="39" borderId="43" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="45" numFmtId="0" fillId="5" borderId="44" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="44" numFmtId="0" fillId="40" borderId="44" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="46" numFmtId="0" fillId="38" borderId="45" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="20" numFmtId="0" fillId="19" borderId="45" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="47" numFmtId="0" fillId="39" borderId="46" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="45" numFmtId="0" fillId="21" borderId="46" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="48" numFmtId="0" fillId="40" borderId="47" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="47" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="49" numFmtId="0" fillId="41" borderId="48" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="46" numFmtId="0" fillId="41" borderId="48" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="50" numFmtId="0" fillId="42" borderId="49" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="47" numFmtId="0" fillId="24" borderId="49" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="51" numFmtId="0" fillId="43" borderId="50" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="48" numFmtId="0" fillId="24" borderId="50" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="52" numFmtId="0" fillId="27" borderId="51" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="49" numFmtId="0" fillId="16" borderId="51" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="20" numFmtId="0" fillId="3" borderId="52" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="50" numFmtId="0" fillId="3" borderId="52" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="53" numFmtId="0" fillId="13" borderId="53" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="51" numFmtId="0" fillId="42" borderId="53" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="54" numFmtId="0" fillId="26" borderId="54" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="52" numFmtId="0" fillId="43" borderId="54" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="55" numFmtId="0" fillId="44" borderId="55" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="34" numFmtId="0" fillId="32" borderId="55" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="56" numFmtId="0" fillId="21" borderId="56" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="14" numFmtId="0" fillId="13" borderId="56" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="57" numFmtId="0" fillId="45" borderId="57" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="53" numFmtId="0" fillId="31" borderId="57" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="32" numFmtId="0" fillId="7" borderId="58" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="54" numFmtId="0" fillId="44" borderId="58" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="58" numFmtId="0" fillId="5" borderId="59" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="55" numFmtId="0" fillId="45" borderId="59" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="27" numFmtId="0" fillId="27" borderId="60" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="56" numFmtId="0" fillId="11" borderId="60" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="45" numFmtId="0" fillId="5" borderId="61" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="57" numFmtId="0" fillId="46" borderId="61" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="59" numFmtId="0" fillId="46" borderId="62" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="58" numFmtId="0" fillId="47" borderId="62" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="60" numFmtId="0" fillId="47" borderId="63" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="59" numFmtId="0" fillId="43" borderId="63" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="61" numFmtId="0" fillId="48" borderId="64" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="60" numFmtId="0" fillId="48" borderId="64" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="62" numFmtId="0" fillId="49" borderId="65" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="61" numFmtId="0" fillId="49" borderId="65" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="63" numFmtId="0" fillId="50" borderId="66" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="62" numFmtId="0" fillId="50" borderId="66" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="64" numFmtId="0" fillId="3" borderId="67" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="63" numFmtId="0" fillId="51" borderId="67" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="65" numFmtId="0" fillId="51" borderId="68" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="64" numFmtId="0" fillId="3" borderId="68" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="66" numFmtId="0" fillId="52" borderId="69" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="65" numFmtId="0" fillId="52" borderId="69" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="67" numFmtId="0" fillId="53" borderId="41" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="66" numFmtId="0" fillId="53" borderId="70" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="68" numFmtId="0" fillId="28" borderId="70" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="67" numFmtId="0" fillId="54" borderId="71" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="69" numFmtId="0" fillId="54" borderId="71" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="68" numFmtId="0" fillId="55" borderId="72" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="29" numFmtId="0" fillId="29" borderId="72" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="69" numFmtId="0" fillId="56" borderId="73" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="70" numFmtId="0" fillId="55" borderId="73" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="70" numFmtId="0" fillId="57" borderId="74" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="12" numFmtId="0" fillId="13" borderId="74" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="71" numFmtId="0" fillId="7" borderId="45" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>

</xml_diff>